<commit_message>
Fix: Remove log auto-scroll, reduce unnecessary page scrolling, improve fill pattern logging
</commit_message>
<xml_diff>
--- a/spreadsheet_fixed_autofixed.xlsx
+++ b/spreadsheet_fixed_autofixed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smart\OneDrive\Desktop\Chatgpt1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9841AF-21E3-4406-9186-1AE529485341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B65CB90-2E3C-4336-A3CE-F25E0C9F52E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="187">
   <si>
     <t>TO BE EXECUTED</t>
   </si>
@@ -195,9 +195,6 @@
     <t>Click Enter Query</t>
   </si>
   <si>
-    <t>Enter Query</t>
-  </si>
-  <si>
     <t xml:space="preserve">Enter Query should be clicked </t>
   </si>
   <si>
@@ -589,6 +586,12 @@
   </si>
   <si>
     <t>Pranitha@25</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter Query </t>
   </si>
 </sst>
 </file>
@@ -1037,7 +1040,7 @@
   <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="A5" sqref="A3:A5"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1145,7 +1148,7 @@
         <v>27</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K3" t="s">
         <v>28</v>
@@ -1168,7 +1171,7 @@
         <v>31</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K4" t="s">
         <v>32</v>
@@ -1188,7 +1191,7 @@
         <v>35</v>
       </c>
       <c r="I5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K5" t="s">
         <v>37</v>
@@ -1208,7 +1211,7 @@
         <v>35</v>
       </c>
       <c r="I6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -1219,13 +1222,13 @@
         <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F8" t="s">
         <v>41</v>
       </c>
       <c r="G8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H8" t="s">
         <v>26</v>
@@ -1234,10 +1237,10 @@
         <v>42</v>
       </c>
       <c r="J8" t="s">
+        <v>117</v>
+      </c>
+      <c r="K8" t="s">
         <v>118</v>
-      </c>
-      <c r="K8" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -1268,16 +1271,16 @@
         <v>48</v>
       </c>
       <c r="G10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H10" t="s">
         <v>35</v>
       </c>
       <c r="I10" t="s">
-        <v>54</v>
+        <v>185</v>
       </c>
       <c r="K10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -1288,17 +1291,17 @@
         <v>49</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H11" t="s">
         <v>35</v>
       </c>
       <c r="I11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
@@ -1309,19 +1312,19 @@
         <v>51</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H12" t="s">
         <v>26</v>
       </c>
       <c r="I12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
@@ -1332,19 +1335,19 @@
         <v>52</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H13" t="s">
         <v>26</v>
       </c>
       <c r="I13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -1352,22 +1355,22 @@
         <v>14</v>
       </c>
       <c r="F14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H14" t="s">
         <v>26</v>
       </c>
       <c r="I14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -1375,22 +1378,22 @@
         <v>14</v>
       </c>
       <c r="F15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H15" t="s">
         <v>26</v>
       </c>
       <c r="I15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
@@ -1398,22 +1401,22 @@
         <v>14</v>
       </c>
       <c r="F16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H16" t="s">
         <v>26</v>
       </c>
       <c r="I16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1421,22 +1424,22 @@
         <v>14</v>
       </c>
       <c r="F17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H17" t="s">
         <v>26</v>
       </c>
       <c r="I17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1444,22 +1447,22 @@
         <v>14</v>
       </c>
       <c r="F18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H18" t="s">
         <v>35</v>
       </c>
       <c r="I18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -1467,22 +1470,22 @@
         <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H19" t="s">
         <v>26</v>
       </c>
       <c r="I19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -1490,22 +1493,22 @@
         <v>14</v>
       </c>
       <c r="F20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H20" t="s">
         <v>26</v>
       </c>
       <c r="I20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1513,19 +1516,19 @@
         <v>14</v>
       </c>
       <c r="F21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H21" t="s">
         <v>35</v>
       </c>
       <c r="I21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K21" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -1533,22 +1536,22 @@
         <v>14</v>
       </c>
       <c r="F22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H22" t="s">
         <v>26</v>
       </c>
       <c r="I22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K22" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -1556,22 +1559,22 @@
         <v>14</v>
       </c>
       <c r="F23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H23" t="s">
         <v>26</v>
       </c>
       <c r="I23" t="s">
+        <v>74</v>
+      </c>
+      <c r="J23" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="J23" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="K23" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -1579,20 +1582,20 @@
         <v>14</v>
       </c>
       <c r="F24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H24" t="s">
         <v>35</v>
       </c>
       <c r="I24" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -1600,19 +1603,19 @@
         <v>14</v>
       </c>
       <c r="F25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H25" t="s">
         <v>35</v>
       </c>
       <c r="I25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -1629,13 +1632,10 @@
         <v>45</v>
       </c>
       <c r="I28" t="s">
+        <v>186</v>
+      </c>
+      <c r="K28" t="s">
         <v>54</v>
-      </c>
-      <c r="J28" t="s">
-        <v>54</v>
-      </c>
-      <c r="K28" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -1646,19 +1646,19 @@
         <v>49</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H29" t="s">
         <v>26</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J29" s="3">
         <v>10381197</v>
       </c>
       <c r="K29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -1669,19 +1669,19 @@
         <v>51</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H30" t="s">
         <v>26</v>
       </c>
       <c r="I30" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="J30" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="J30" s="3" t="s">
+      <c r="K30" t="s">
         <v>61</v>
-      </c>
-      <c r="K30" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -1692,19 +1692,19 @@
         <v>52</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H31" t="s">
         <v>26</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J31" s="3">
         <v>120</v>
       </c>
       <c r="K31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -1712,10 +1712,10 @@
         <v>50</v>
       </c>
       <c r="F32" t="s">
+        <v>65</v>
+      </c>
+      <c r="G32" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="H32" t="s">
         <v>35</v>
@@ -1725,7 +1725,7 @@
       </c>
       <c r="J32" s="3"/>
       <c r="K32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
@@ -1733,22 +1733,22 @@
         <v>50</v>
       </c>
       <c r="F33" t="s">
+        <v>68</v>
+      </c>
+      <c r="G33" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="H33" t="s">
         <v>26</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J33" s="3">
         <v>100</v>
       </c>
       <c r="K33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
@@ -1756,22 +1756,22 @@
         <v>50</v>
       </c>
       <c r="F34" t="s">
+        <v>72</v>
+      </c>
+      <c r="G34" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="H34" t="s">
         <v>26</v>
       </c>
       <c r="I34" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="J34" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="J34" s="3" t="s">
+      <c r="K34" t="s">
         <v>76</v>
-      </c>
-      <c r="K34" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
@@ -1779,22 +1779,22 @@
         <v>50</v>
       </c>
       <c r="F35" t="s">
+        <v>77</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="H35" t="s">
         <v>26</v>
       </c>
       <c r="I35" t="s">
+        <v>79</v>
+      </c>
+      <c r="J35" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="J35" s="3" t="s">
+      <c r="K35" t="s">
         <v>81</v>
-      </c>
-      <c r="K35" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
@@ -1802,10 +1802,10 @@
         <v>50</v>
       </c>
       <c r="F36" t="s">
+        <v>82</v>
+      </c>
+      <c r="G36" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="H36" t="s">
         <v>35</v>
@@ -1815,7 +1815,7 @@
       </c>
       <c r="J36" s="3"/>
       <c r="K36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
@@ -1829,31 +1829,31 @@
         <v>50</v>
       </c>
       <c r="B38" t="s">
+        <v>85</v>
+      </c>
+      <c r="D38" t="s">
         <v>86</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>87</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>88</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" s="6" t="s">
         <v>89</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>90</v>
       </c>
       <c r="H38" t="s">
         <v>21</v>
       </c>
       <c r="I38" t="s">
+        <v>90</v>
+      </c>
+      <c r="J38" t="s">
+        <v>90</v>
+      </c>
+      <c r="K38" t="s">
         <v>91</v>
-      </c>
-      <c r="J38" t="s">
-        <v>91</v>
-      </c>
-      <c r="K38" t="s">
-        <v>92</v>
       </c>
       <c r="M38" s="12"/>
       <c r="N38" s="12"/>
@@ -1863,19 +1863,19 @@
         <v>50</v>
       </c>
       <c r="F39" t="s">
+        <v>92</v>
+      </c>
+      <c r="G39" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>94</v>
       </c>
       <c r="H39" t="s">
         <v>45</v>
       </c>
       <c r="I39" t="s">
+        <v>94</v>
+      </c>
+      <c r="K39" t="s">
         <v>95</v>
-      </c>
-      <c r="K39" t="s">
-        <v>96</v>
       </c>
       <c r="M39" s="12"/>
       <c r="N39" s="12"/>
@@ -1885,20 +1885,20 @@
         <v>50</v>
       </c>
       <c r="F40" t="s">
+        <v>96</v>
+      </c>
+      <c r="G40" s="6" t="s">
         <v>97</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>98</v>
       </c>
       <c r="H40" t="s">
         <v>45</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J40" s="8"/>
       <c r="K40" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M40" s="12"/>
       <c r="N40" s="12"/>
@@ -1908,19 +1908,19 @@
         <v>50</v>
       </c>
       <c r="F41" t="s">
+        <v>100</v>
+      </c>
+      <c r="G41" s="6" t="s">
         <v>101</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>102</v>
       </c>
       <c r="H41" t="s">
         <v>45</v>
       </c>
       <c r="I41" t="s">
+        <v>102</v>
+      </c>
+      <c r="K41" t="s">
         <v>103</v>
-      </c>
-      <c r="K41" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
@@ -1928,19 +1928,19 @@
         <v>50</v>
       </c>
       <c r="F42" t="s">
+        <v>104</v>
+      </c>
+      <c r="G42" s="6" t="s">
         <v>105</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>106</v>
       </c>
       <c r="H42" t="s">
         <v>45</v>
       </c>
       <c r="I42" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="K42" t="s">
         <v>107</v>
-      </c>
-      <c r="K42" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.3">
@@ -1948,19 +1948,19 @@
         <v>50</v>
       </c>
       <c r="F43" t="s">
+        <v>108</v>
+      </c>
+      <c r="G43" s="6" t="s">
         <v>109</v>
-      </c>
-      <c r="G43" s="6" t="s">
-        <v>110</v>
       </c>
       <c r="H43" t="s">
         <v>45</v>
       </c>
       <c r="I43" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="K43" t="s">
         <v>111</v>
-      </c>
-      <c r="K43" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.3">
@@ -1968,19 +1968,19 @@
         <v>50</v>
       </c>
       <c r="F44" t="s">
+        <v>112</v>
+      </c>
+      <c r="G44" s="6" t="s">
         <v>113</v>
-      </c>
-      <c r="G44" s="6" t="s">
-        <v>114</v>
       </c>
       <c r="H44" t="s">
         <v>45</v>
       </c>
       <c r="I44" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="K44" t="s">
         <v>115</v>
-      </c>
-      <c r="K44" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated assistant code and test results
</commit_message>
<xml_diff>
--- a/spreadsheet_fixed_autofixed.xlsx
+++ b/spreadsheet_fixed_autofixed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smart\OneDrive\Desktop\Chatgpt1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37558519-BBC4-42E4-8548-942E08A9EC5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53A46E8-9E86-4754-8593-6AE2BFCEABB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2508" yWindow="2508" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="185">
   <si>
     <t>TO BE EXECUTED</t>
   </si>
@@ -586,13 +586,7 @@
     <t>Pranitha@25</t>
   </si>
   <si>
-    <t>New</t>
-  </si>
-  <si>
     <t xml:space="preserve">Enter Query </t>
-  </si>
-  <si>
-    <t>Click New</t>
   </si>
 </sst>
 </file>
@@ -1040,8 +1034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="79" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="79" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1272,7 +1266,7 @@
         <v>48</v>
       </c>
       <c r="G10" t="s">
-        <v>186</v>
+        <v>53</v>
       </c>
       <c r="H10" t="s">
         <v>35</v>
@@ -1633,7 +1627,7 @@
         <v>45</v>
       </c>
       <c r="I28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K28" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
Reduce logging verbosity and deploy universal iframe automation system
- Disable logWindowSummary and logFrameStructure by default to reduce noise
- Remove individual overlay search candidate logging
- Remove PRIORITY 1 overlay search messages
- Implement universal iframe discovery (no hardcoding)
- Add dynamic element finding via CSS locators and text matching
- Maintain multi-window support
- All test data from Excel (100% dynamic)
- No XPath - using CSS selectors instead
- TypeScript compiles with zero errors
</commit_message>
<xml_diff>
--- a/spreadsheet_fixed_autofixed.xlsx
+++ b/spreadsheet_fixed_autofixed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smart\OneDrive\Desktop\Chatgpt1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495D0AE4-9C03-44D2-8A6B-898F3B85E9A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDE284C-E3E3-4ACE-A84B-75B66CF6E23C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1038,7 +1038,7 @@
   <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="79" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1407,7 +1407,7 @@
       <c r="H16" t="s">
         <v>26</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="5" t="s">
         <v>139</v>
       </c>
       <c r="J16" s="3" t="s">

</xml_diff>

<commit_message>
Enhanced automation assistant: Add cursor pointer indicators, hierarchical dropdown navigation, hover-reveal support, and improved element detection strategies
</commit_message>
<xml_diff>
--- a/spreadsheet_fixed_autofixed.xlsx
+++ b/spreadsheet_fixed_autofixed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smart\OneDrive\Desktop\Chatgpt1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C8BC996-AE88-4EB6-817E-E9AEFE5EC852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1450FBC8-69F1-439A-95AD-EB18376377A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="155">
   <si>
     <t>TO BE EXECUTED</t>
   </si>
@@ -284,99 +284,6 @@
   </si>
   <si>
     <t xml:space="preserve">Save and Select accept should be clicked </t>
-  </si>
-  <si>
-    <t>TS002</t>
-  </si>
-  <si>
-    <t>TS111TC001</t>
-  </si>
-  <si>
-    <t>Flipkart</t>
-  </si>
-  <si>
-    <t>TS111TC001TSP001</t>
-  </si>
-  <si>
-    <t>Open the url</t>
-  </si>
-  <si>
-    <t>https://www.flipkart.com/</t>
-  </si>
-  <si>
-    <t>URL should be opened</t>
-  </si>
-  <si>
-    <t>TS111TC001TSP002</t>
-  </si>
-  <si>
-    <t>Click Login</t>
-  </si>
-  <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>Login should be clicked</t>
-  </si>
-  <si>
-    <t>TS111TC001TSP003</t>
-  </si>
-  <si>
-    <t>Click Men</t>
-  </si>
-  <si>
-    <t>Men</t>
-  </si>
-  <si>
-    <t>Men should be clicked</t>
-  </si>
-  <si>
-    <t>TS111TC001TSP004</t>
-  </si>
-  <si>
-    <t>Click Running Shoes</t>
-  </si>
-  <si>
-    <t>Running Shoes</t>
-  </si>
-  <si>
-    <t>Running shoes should be clicked</t>
-  </si>
-  <si>
-    <t>TS111TC001TSP005</t>
-  </si>
-  <si>
-    <t>Click COLOR</t>
-  </si>
-  <si>
-    <t>COLOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COLOR should be clicked </t>
-  </si>
-  <si>
-    <t>TS111TC001TSP006</t>
-  </si>
-  <si>
-    <t>Click Blue</t>
-  </si>
-  <si>
-    <t>Blue</t>
-  </si>
-  <si>
-    <t>Blue should be selected</t>
-  </si>
-  <si>
-    <t>TS111TC001TSP007</t>
-  </si>
-  <si>
-    <t>Click BestSeller</t>
-  </si>
-  <si>
-    <t>BestSeller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Best seller product should be clicked </t>
   </si>
   <si>
     <t>Enter STDCIF in the Function Id</t>
@@ -1037,8 +944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="79" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="79" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1120,10 +1027,10 @@
         <v>21</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>185</v>
+        <v>154</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>185</v>
+        <v>154</v>
       </c>
       <c r="K2" t="s">
         <v>22</v>
@@ -1146,7 +1053,7 @@
         <v>26</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>179</v>
+        <v>148</v>
       </c>
       <c r="K3" t="s">
         <v>27</v>
@@ -1169,7 +1076,7 @@
         <v>30</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>180</v>
+        <v>149</v>
       </c>
       <c r="K4" t="s">
         <v>31</v>
@@ -1189,7 +1096,7 @@
         <v>34</v>
       </c>
       <c r="I5" t="s">
-        <v>177</v>
+        <v>146</v>
       </c>
       <c r="K5" t="s">
         <v>36</v>
@@ -1209,7 +1116,7 @@
         <v>34</v>
       </c>
       <c r="I6" t="s">
-        <v>178</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -1220,13 +1127,13 @@
         <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>145</v>
+        <v>114</v>
       </c>
       <c r="F8" t="s">
         <v>40</v>
       </c>
       <c r="G8" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="H8" t="s">
         <v>25</v>
@@ -1235,10 +1142,10 @@
         <v>41</v>
       </c>
       <c r="J8" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="K8" t="s">
-        <v>117</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -1269,16 +1176,16 @@
         <v>47</v>
       </c>
       <c r="G10" t="s">
-        <v>183</v>
+        <v>152</v>
       </c>
       <c r="H10" t="s">
         <v>34</v>
       </c>
       <c r="I10" t="s">
-        <v>182</v>
+        <v>151</v>
       </c>
       <c r="K10" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -1289,17 +1196,17 @@
         <v>48</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="H11" t="s">
         <v>34</v>
       </c>
       <c r="I11" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" t="s">
-        <v>176</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
@@ -1310,19 +1217,19 @@
         <v>50</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="H12" t="s">
         <v>25</v>
       </c>
       <c r="I12" t="s">
-        <v>134</v>
+        <v>103</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="K12" t="s">
-        <v>162</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
@@ -1333,19 +1240,19 @@
         <v>51</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>120</v>
+        <v>89</v>
       </c>
       <c r="H13" t="s">
         <v>25</v>
       </c>
       <c r="I13" t="s">
-        <v>135</v>
+        <v>104</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>157</v>
+        <v>126</v>
       </c>
       <c r="K13" t="s">
-        <v>163</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -1356,19 +1263,19 @@
         <v>64</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>121</v>
+        <v>90</v>
       </c>
       <c r="H14" t="s">
         <v>25</v>
       </c>
       <c r="I14" t="s">
-        <v>136</v>
+        <v>105</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
       <c r="K14" t="s">
-        <v>164</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -1379,19 +1286,19 @@
         <v>67</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>123</v>
+        <v>92</v>
       </c>
       <c r="H15" t="s">
         <v>25</v>
       </c>
       <c r="I15" t="s">
-        <v>137</v>
+        <v>106</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
       <c r="K15" t="s">
-        <v>165</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
@@ -1402,19 +1309,19 @@
         <v>71</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>124</v>
+        <v>93</v>
       </c>
       <c r="H16" t="s">
         <v>25</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>138</v>
+        <v>107</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>126</v>
+        <v>95</v>
       </c>
       <c r="K16" t="s">
-        <v>166</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1425,19 +1332,19 @@
         <v>76</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>125</v>
+        <v>94</v>
       </c>
       <c r="H17" t="s">
         <v>25</v>
       </c>
       <c r="I17" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>126</v>
+        <v>95</v>
       </c>
       <c r="K17" t="s">
-        <v>167</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1448,17 +1355,17 @@
         <v>81</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>127</v>
+        <v>96</v>
       </c>
       <c r="H18" t="s">
         <v>34</v>
       </c>
       <c r="I18" t="s">
-        <v>184</v>
+        <v>153</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" t="s">
-        <v>168</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -1466,22 +1373,22 @@
         <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>146</v>
+        <v>115</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>128</v>
+        <v>97</v>
       </c>
       <c r="H19" t="s">
         <v>25</v>
       </c>
       <c r="I19" t="s">
-        <v>141</v>
+        <v>110</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
       <c r="K19" t="s">
-        <v>169</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -1489,22 +1396,22 @@
         <v>14</v>
       </c>
       <c r="F20" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="H20" t="s">
         <v>25</v>
       </c>
       <c r="I20" t="s">
-        <v>140</v>
+        <v>109</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>130</v>
+        <v>99</v>
       </c>
       <c r="K20" t="s">
-        <v>170</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1512,19 +1419,19 @@
         <v>14</v>
       </c>
       <c r="F21" t="s">
-        <v>148</v>
+        <v>117</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>153</v>
+        <v>122</v>
       </c>
       <c r="H21" t="s">
         <v>34</v>
       </c>
       <c r="I21" t="s">
-        <v>159</v>
+        <v>128</v>
       </c>
       <c r="K21" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -1532,10 +1439,10 @@
         <v>14</v>
       </c>
       <c r="F22" t="s">
-        <v>149</v>
+        <v>118</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>154</v>
+        <v>123</v>
       </c>
       <c r="H22" t="s">
         <v>25</v>
@@ -1544,10 +1451,10 @@
         <v>69</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>131</v>
+        <v>100</v>
       </c>
       <c r="K22" t="s">
-        <v>173</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -1555,10 +1462,10 @@
         <v>14</v>
       </c>
       <c r="F23" t="s">
-        <v>150</v>
+        <v>119</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>132</v>
+        <v>101</v>
       </c>
       <c r="H23" t="s">
         <v>25</v>
@@ -1570,7 +1477,7 @@
         <v>74</v>
       </c>
       <c r="K23" t="s">
-        <v>172</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -1578,20 +1485,20 @@
         <v>14</v>
       </c>
       <c r="F24" t="s">
-        <v>151</v>
+        <v>120</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>142</v>
+        <v>111</v>
       </c>
       <c r="H24" t="s">
         <v>34</v>
       </c>
       <c r="I24" t="s">
-        <v>160</v>
+        <v>129</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" t="s">
-        <v>174</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -1599,24 +1506,24 @@
         <v>14</v>
       </c>
       <c r="F25" t="s">
-        <v>155</v>
+        <v>124</v>
       </c>
       <c r="G25" t="s">
-        <v>143</v>
+        <v>112</v>
       </c>
       <c r="H25" t="s">
         <v>34</v>
       </c>
       <c r="I25" t="s">
+        <v>113</v>
+      </c>
+      <c r="K25" t="s">
         <v>144</v>
-      </c>
-      <c r="K25" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="F28" t="s">
         <v>47</v>
@@ -1628,7 +1535,7 @@
         <v>44</v>
       </c>
       <c r="I28" t="s">
-        <v>181</v>
+        <v>150</v>
       </c>
       <c r="K28" t="s">
         <v>53</v>
@@ -1636,7 +1543,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="F29" t="s">
         <v>48</v>
@@ -1659,7 +1566,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="F30" t="s">
         <v>50</v>
@@ -1682,7 +1589,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="F31" t="s">
         <v>51</v>
@@ -1705,7 +1612,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="F32" t="s">
         <v>64</v>
@@ -1726,7 +1633,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="F33" t="s">
         <v>67</v>
@@ -1749,7 +1656,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="F34" t="s">
         <v>71</v>
@@ -1772,7 +1679,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="F35" t="s">
         <v>76</v>
@@ -1795,7 +1702,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="F36" t="s">
         <v>81</v>
@@ -1821,163 +1728,36 @@
       <c r="N37" s="12"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>49</v>
-      </c>
-      <c r="B38" t="s">
-        <v>84</v>
-      </c>
-      <c r="D38" t="s">
-        <v>85</v>
-      </c>
-      <c r="E38" t="s">
-        <v>86</v>
-      </c>
-      <c r="F38" t="s">
-        <v>87</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="H38" t="s">
-        <v>21</v>
-      </c>
-      <c r="I38" t="s">
-        <v>89</v>
-      </c>
-      <c r="J38" t="s">
-        <v>89</v>
-      </c>
-      <c r="K38" t="s">
-        <v>90</v>
-      </c>
+      <c r="G38" s="6"/>
       <c r="M38" s="12"/>
       <c r="N38" s="12"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>49</v>
-      </c>
-      <c r="F39" t="s">
-        <v>91</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="H39" t="s">
-        <v>44</v>
-      </c>
-      <c r="I39" t="s">
-        <v>93</v>
-      </c>
-      <c r="K39" t="s">
-        <v>94</v>
-      </c>
+      <c r="G39" s="6"/>
       <c r="M39" s="12"/>
       <c r="N39" s="12"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>49</v>
-      </c>
-      <c r="F40" t="s">
-        <v>95</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="H40" t="s">
-        <v>44</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>97</v>
-      </c>
+      <c r="G40" s="6"/>
+      <c r="I40" s="1"/>
       <c r="J40" s="8"/>
-      <c r="K40" t="s">
-        <v>98</v>
-      </c>
       <c r="M40" s="12"/>
       <c r="N40" s="12"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>49</v>
-      </c>
-      <c r="F41" t="s">
-        <v>99</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="H41" t="s">
-        <v>44</v>
-      </c>
-      <c r="I41" t="s">
-        <v>101</v>
-      </c>
-      <c r="K41" t="s">
-        <v>102</v>
-      </c>
+      <c r="G41" s="6"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>49</v>
-      </c>
-      <c r="F42" t="s">
-        <v>103</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="H42" t="s">
-        <v>44</v>
-      </c>
-      <c r="I42" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="K42" t="s">
-        <v>106</v>
-      </c>
+      <c r="G42" s="6"/>
+      <c r="I42" s="9"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>49</v>
-      </c>
-      <c r="F43" t="s">
-        <v>107</v>
-      </c>
-      <c r="G43" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H43" t="s">
-        <v>44</v>
-      </c>
-      <c r="I43" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="K43" t="s">
-        <v>110</v>
-      </c>
+      <c r="G43" s="6"/>
+      <c r="I43" s="9"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>49</v>
-      </c>
-      <c r="F44" t="s">
-        <v>111</v>
-      </c>
-      <c r="G44" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="H44" t="s">
-        <v>44</v>
-      </c>
-      <c r="I44" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="K44" t="s">
-        <v>114</v>
-      </c>
+      <c r="G44" s="6"/>
+      <c r="I44" s="9"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G45" s="6"/>

</xml_diff>